<commit_message>
No need for asking number, only if the user has his phone number and added by admin. others are not allowed for use.
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -19,6 +19,17 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t xml:space="preserve">Phone Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User ID</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
@@ -29,6 +40,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -88,8 +100,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -216,24 +232,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.26"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>907510905</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
+        <v>907510905</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
         <v>938636344</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added option to select category, then it will go for the nomenclature to display what you want.
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,6 +477,14 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>@adsad</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>